<commit_message>
sync up with latest in nexial-core
</commit_message>
<xml_diff>
--- a/src/test/resources/org/nexial/core/ExecutionInputPrepTest_test1.data.xlsx
+++ b/src/test/resources/org/nexial/core/ExecutionInputPrepTest_test1.data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10530"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-core/src/test/resources/com/ep/qa/sentry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/org/nexial/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6A6E2C-5E8A-104B-A6DB-5869C6E06918}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="31460" windowWidth="25600" xWindow="25600" yWindow="440"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scenario1" r:id="rId1" sheetId="3"/>
-    <sheet name="scenario2" r:id="rId2" sheetId="4"/>
+    <sheet name="scenario1" sheetId="3" r:id="rId1"/>
+    <sheet name="scenario2" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,20 +29,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>sentry.pollWaitMs</t>
-  </si>
-  <si>
     <t>800</t>
   </si>
   <si>
-    <t>sentry.textDelim</t>
-  </si>
-  <si>
     <t>,</t>
   </si>
   <si>
@@ -57,39 +52,18 @@
     <t>Value2</t>
   </si>
   <si>
-    <t>sentry.scope.mailTo</t>
-  </si>
-  <si>
-    <t>sentry.scope.executionMode</t>
-  </si>
-  <si>
     <t>local</t>
   </si>
   <si>
-    <t>sentry.scope.fallbackToPrevious</t>
-  </si>
-  <si>
-    <t>sentry.scope.iteration</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>sentry.delayBetweenStepsMs</t>
-  </si>
-  <si>
     <t>600</t>
   </si>
   <si>
-    <t>sentry.failFast</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
-    <t>sentry.verbose</t>
-  </si>
-  <si>
     <t>Value1a</t>
   </si>
   <si>
@@ -102,9 +76,6 @@
     <t>jumbotron@tiny.corp</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>nexial.scope.executionMode</t>
   </si>
   <si>
@@ -114,9 +85,6 @@
     <t>nexial.scope.iteration</t>
   </si>
   <si>
-    <t>nexial.scope.mailTo</t>
-  </si>
-  <si>
     <t>nexial.delayBetweenStepsMs</t>
   </si>
   <si>
@@ -130,14 +98,19 @@
   </si>
   <si>
     <t>nexial.verbose</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>nexial.mailTo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,15 +122,18 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -169,6 +145,7 @@
       <i/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -220,43 +197,43 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="5" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -438,10 +415,13 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -452,10 +432,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -490,7 +470,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -525,7 +505,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -619,21 +599,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -650,7 +630,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -702,39 +682,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AAB11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AAA11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
-      <selection sqref="A1:B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="28.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="2" width="21.1640625" collapsed="false"/>
-    <col min="3" max="27" customWidth="true" style="3" width="21.1640625" collapsed="false"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="false"/>
+    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="2" customWidth="1"/>
+    <col min="3" max="27" width="21.1640625" style="3" customWidth="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:703" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -742,154 +722,154 @@
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:703">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="HA4" s="6"/>
       <c r="AAA4" s="6"/>
     </row>
-    <row r="5" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
-    <row r="10" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
-    <row r="11" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="HA11" s="4"/>
       <c r="AAA11" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0" sheet="1"/>
+  <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule dxfId="13" operator="beginsWith" priority="5" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="13" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="12" operator="beginsWith" priority="6" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="12" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="11" priority="7" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B1048576 B1">
-    <cfRule dxfId="10" priority="3" type="expression">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
-    <cfRule dxfId="9" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="4">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule dxfId="8" priority="1" type="expression">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
-    <cfRule dxfId="7" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AAB8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AAA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="28.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="2" width="21.1640625" collapsed="false"/>
-    <col min="3" max="27" customWidth="true" style="3" width="21.1640625" collapsed="false"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="false"/>
+    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="2" customWidth="1"/>
+    <col min="3" max="27" width="21.1640625" style="3" customWidth="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:703" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -897,39 +877,39 @@
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:703">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="HA4" s="6"/>
       <c r="AAA4" s="6"/>
     </row>
-    <row r="5" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -937,59 +917,59 @@
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="1:703" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0" sheet="1"/>
+  <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule dxfId="6" operator="beginsWith" priority="5" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="5" operator="beginsWith" priority="6" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="5" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="4" priority="7" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B1048576">
-    <cfRule dxfId="3" priority="3" type="expression">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
-    <cfRule dxfId="2" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule dxfId="1" priority="1" type="expression">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
-    <cfRule dxfId="0" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>